<commit_message>
generalize grid spreadsheet to 5 motors
+ read motor identity from header
+ remove columns identifying motors
+ up spreadsheet version to 17
+ cleanup commented lines from linescans.py
</commit_message>
<xml_diff>
--- a/startup/xlsx/lakeshore.xlsx
+++ b/startup/xlsx/lakeshore.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="lakeshore1" sheetId="1" state="visible" r:id="rId2"/>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="78">
   <si>
     <t xml:space="preserve">LakeShore</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t xml:space="preserve">added resonant reflectivity spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select grid motors by setting position column headers</t>
   </si>
 </sst>
 </file>
@@ -1549,9 +1552,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1625040</xdr:colOff>
+      <xdr:colOff>1624680</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1561,7 +1564,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5185800" y="6296400"/>
-          <a:ext cx="6654960" cy="1783800"/>
+          <a:ext cx="6655320" cy="1783440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1794,9 +1797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1355400</xdr:colOff>
+      <xdr:colOff>1355040</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1806,7 +1809,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4789080" y="7347240"/>
-          <a:ext cx="6654960" cy="1784160"/>
+          <a:ext cx="6655320" cy="1783800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2039,9 +2042,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>824040</xdr:colOff>
+      <xdr:colOff>823680</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2051,7 +2054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6654600" cy="1784160"/>
+          <a:ext cx="6654960" cy="1783800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2284,9 +2287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>853200</xdr:colOff>
+      <xdr:colOff>852840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2296,7 +2299,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6652800" cy="1784160"/>
+          <a:ext cx="6653160" cy="1783800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2529,9 +2532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>774720</xdr:colOff>
+      <xdr:colOff>774360</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2541,7 +2544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6654960" cy="1784160"/>
+          <a:ext cx="6655320" cy="1783800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2770,15 +2773,15 @@
   </sheetPr>
   <dimension ref="B1:AF14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I6" activeCellId="1" sqref="A3 I6"/>
+      <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -2836,7 +2839,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 16</v>
+        <v>Version: 17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -3416,10 +3419,6 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I13:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
@@ -3436,16 +3435,20 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I12" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
-      <formula1>"unfocused,focused"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I12" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I13:I14" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3473,10 +3476,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I12" activeCellId="1" sqref="A3 I12"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -3535,7 +3538,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 16</v>
+        <v>Version: 17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -4138,21 +4141,21 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6" type="list">
-      <formula1>"unfocused,focused"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
-      <formula1>"True,False"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
@@ -4183,10 +4186,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I12" activeCellId="1" sqref="A3 I12"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -4243,7 +4246,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 16</v>
+        <v>Version: 17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -4883,10 +4886,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I12" activeCellId="1" sqref="A3 I12"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -4943,7 +4946,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 16</v>
+        <v>Version: 17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -5583,10 +5586,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I7" activeCellId="1" sqref="A3 I7"/>
+      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -5643,7 +5646,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 16</v>
+        <v>Version: 17</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -6276,13 +6279,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -6301,7 +6304,7 @@
     <row r="3" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="n">
         <f aca="false">MAX(A6:A41)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6433,6 +6436,14 @@
       </c>
       <c r="B20" s="0" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>